<commit_message>
3 out of 3 correct 68 recall
</commit_message>
<xml_diff>
--- a/predictionsFour.xlsx
+++ b/predictionsFour.xlsx
@@ -498,7 +498,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -514,7 +514,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -554,7 +554,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -650,7 +650,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -722,7 +722,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -754,7 +754,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -770,7 +770,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -802,7 +802,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -834,7 +834,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">

</xml_diff>

<commit_message>
possible features to use
</commit_message>
<xml_diff>
--- a/predictionsFour.xlsx
+++ b/predictionsFour.xlsx
@@ -762,7 +762,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -802,7 +802,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1082,7 +1082,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -1354,7 +1354,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -1490,7 +1490,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133">
@@ -1506,7 +1506,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -2226,7 +2226,7 @@
         <v>223</v>
       </c>
       <c r="B224" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="225">
@@ -2498,7 +2498,7 @@
         <v>257</v>
       </c>
       <c r="B258" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="259">
@@ -2906,7 +2906,7 @@
         <v>308</v>
       </c>
       <c r="B309" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="310">
@@ -2954,7 +2954,7 @@
         <v>314</v>
       </c>
       <c r="B315" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="316">
@@ -3402,7 +3402,7 @@
         <v>370</v>
       </c>
       <c r="B371" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="372">
@@ -3690,7 +3690,7 @@
         <v>406</v>
       </c>
       <c r="B407" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="408">
@@ -4050,7 +4050,7 @@
         <v>451</v>
       </c>
       <c r="B452" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="453">
@@ -4130,7 +4130,7 @@
         <v>461</v>
       </c>
       <c r="B462" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="463">
@@ -4170,7 +4170,7 @@
         <v>466</v>
       </c>
       <c r="B467" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="468">
@@ -4930,7 +4930,7 @@
         <v>561</v>
       </c>
       <c r="B562" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="563">

</xml_diff>